<commit_message>
Update Plan de Control y Seguimiento.xlsx
</commit_message>
<xml_diff>
--- a/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
+++ b/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\GitHub\portafolio\Documentación (Avances)\Primera Iteración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F59AC9E-9D42-4095-A386-EE6674261665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58481C7-A9C4-483B-8098-A28E2B464374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Iteración" sheetId="1" r:id="rId1"/>
@@ -1024,8 +1024,8 @@
   </sheetPr>
   <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -1482,7 +1482,9 @@
       <c r="F27" s="56">
         <v>43755</v>
       </c>
-      <c r="G27" s="52"/>
+      <c r="G27" s="61">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="11"/>
@@ -2117,7 +2119,7 @@
   </sheetPr>
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualización porcentaje de avance diagramas de actividad
Manuel Torres
</commit_message>
<xml_diff>
--- a/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
+++ b/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\GitHub\portafolio\Documentación (Avances)\Primera Iteración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58481C7-A9C4-483B-8098-A28E2B464374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE0636D-D624-4264-A070-A3BCA64E0B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,8 +1024,8 @@
   </sheetPr>
   <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -1483,7 +1483,7 @@
         <v>43755</v>
       </c>
       <c r="G27" s="61">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="28" spans="1:7">

</xml_diff>

<commit_message>
Actualización porcentaje de avance matriz raci . Renzo espeleta ( 100%)
</commit_message>
<xml_diff>
--- a/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
+++ b/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\GitHub\portafolio\Documentación (Avances)\Primera Iteración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE0636D-D624-4264-A070-A3BCA64E0B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880D6651-750C-4E66-8C41-91D8CB4E391E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,8 +1024,8 @@
   </sheetPr>
   <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -1144,8 +1144,8 @@
       <c r="C10" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="58" t="s">
-        <v>73</v>
+      <c r="D10" s="53" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="55">
         <v>43752</v>
@@ -1153,7 +1153,9 @@
       <c r="F10" s="56">
         <v>43755</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="61">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="51" t="s">

</xml_diff>

<commit_message>
Actualización porcentaje de avances  diagrama de actividades
</commit_message>
<xml_diff>
--- a/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
+++ b/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\GitHub\portafolio\Documentación (Avances)\Primera Iteración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880D6651-750C-4E66-8C41-91D8CB4E391E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD57639C-015B-4266-B4D3-3D786B2EE658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,8 +1024,8 @@
   </sheetPr>
   <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -1485,7 +1485,7 @@
         <v>43755</v>
       </c>
       <c r="G27" s="61">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="28" spans="1:7">

</xml_diff>

<commit_message>
Actualizar porcentaje de avance diagrama de actividades
</commit_message>
<xml_diff>
--- a/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
+++ b/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\GitHub\portafolio\Documentación (Avances)\Primera Iteración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD57639C-015B-4266-B4D3-3D786B2EE658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F07E03E-03AB-449F-AC18-E223EDB773A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1485,7 +1485,7 @@
         <v>43755</v>
       </c>
       <c r="G27" s="61">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="28" spans="1:7">

</xml_diff>